<commit_message>
ajuste uucc y template word
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\30.coordinacion-de-carrera\seguimiento\LGTI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C68570-11B3-473D-937E-42259790E62A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A286FF0-0DA2-492C-B117-7F2530741E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="162">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -678,7 +678,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,6 +715,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -740,7 +752,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -805,6 +817,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,12 +844,8 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="5" xr:uid="{05F99610-EFDD-41FA-9067-2D9EACE38C58}"/>
@@ -866,6 +880,192 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1227,192 +1427,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4442,29 +4456,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP(A5,DEPIT!A4:J43,7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="36">
       <calculatedColumnFormula>F5+(365*2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="35">
       <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="16">
+    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="34">
       <calculatedColumnFormula>G5 - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="33">
       <calculatedColumnFormula>IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="14">
+    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="32">
       <calculatedColumnFormula>CONCATENATE(Tabla7[[#This Row],[CÓDIGO]]," - ",Tabla7[[#This Row],[ASIGNATURA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4473,23 +4487,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A4:J49" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J49">
     <sortCondition ref="A5:A49"/>
     <sortCondition descending="1" ref="G5:G49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4827,10 +4841,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="28"/>
+      <c r="K2" s="30"/>
       <c r="L2" s="13">
         <f>GETPIVOTDATA("FULLNAME",$A$4)</f>
         <v>43</v>
@@ -5248,8 +5262,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5269,42 +5283,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
@@ -6981,10 +6995,10 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="31"/>
+      <c r="B50" s="33"/>
     </row>
     <row r="51" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
@@ -7020,84 +7034,84 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I5:I47">
-    <cfRule type="cellIs" dxfId="44" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="42" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H47">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="1901">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1901">
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7143,22 +7157,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
@@ -8025,10 +8039,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A2:G1048560"/>
+  <dimension ref="A2:G1048558"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8041,49 +8055,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="28" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="7">
+      <c r="A6" s="37">
         <v>6002</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -8092,12 +8106,10 @@
       <c r="C6" s="9">
         <v>45000</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="7">
+      <c r="A7" s="37">
         <v>6003</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -8106,12 +8118,10 @@
       <c r="C7" s="9">
         <v>45000</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="7">
+      <c r="A8" s="37">
         <v>6004</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -8120,27 +8130,25 @@
       <c r="C8" s="9">
         <v>45000</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="7">
-        <v>6005</v>
+      <c r="A9" s="37">
+        <v>6004</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C9" s="9">
-        <v>45000</v>
+        <v>45001</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="7">
-        <v>6009</v>
+      <c r="A10" s="37">
+        <v>6005</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>150</v>
@@ -8148,13 +8156,11 @@
       <c r="C10" s="9">
         <v>45000</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="7">
-        <v>6011</v>
+      <c r="A11" s="37">
+        <v>6009</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>150</v>
@@ -8162,13 +8168,11 @@
       <c r="C11" s="9">
         <v>45000</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="7">
-        <v>6013</v>
+      <c r="A12" s="37">
+        <v>6011</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>150</v>
@@ -8176,74 +8180,339 @@
       <c r="C12" s="9">
         <v>45000</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="7">
-        <v>6031</v>
+      <c r="A13" s="38">
+        <v>6012</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C13" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="37">
+        <v>6013</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="9">
         <v>45000</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="38">
+        <v>6014</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="38">
+        <v>6015</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="38">
+        <v>6015</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>160</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="38">
+        <v>6017</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="38">
+        <v>6018</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="38">
+        <v>6020</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="38">
+        <v>6024</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="38">
+        <v>6026</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="38">
+        <v>6027</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="38">
+        <v>6028</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="38">
+        <v>6029</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="37">
+        <v>6031</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="38">
+        <v>6032</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="38">
+        <v>6033</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" s="38">
+        <v>6034</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" s="38">
+        <v>6035</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" s="38">
+        <v>6036</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A32" s="38">
+        <v>6037</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" s="38">
+        <v>6038</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" s="38">
+        <v>6040</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" s="38">
+        <v>6041</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" s="38">
+        <v>6042</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" s="38">
+        <v>6043</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="1048551" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048551" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="1048552" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048552" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
     <row r="1048553" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048553" s="7" t="s">
-        <v>149</v>
+      <c r="A1048553" s="29" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="1048554" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048554" s="36" t="s">
-        <v>150</v>
+      <c r="A1048554" s="29" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="1048555" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048555" s="36" t="s">
-        <v>151</v>
+      <c r="A1048555" s="29" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="1048556" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048556" s="36" t="s">
-        <v>152</v>
+      <c r="A1048556" s="29" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="1048557" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048557" s="36" t="s">
-        <v>153</v>
+      <c r="A1048557" s="29" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="1048558" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048558" s="36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="1048559" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048559" s="36" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="1048560" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048560" s="36" t="s">
+      <c r="A1048558" s="29" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F13">
-    <sortCondition ref="A6:A13"/>
-    <sortCondition ref="C6:C13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F37">
+    <sortCondition ref="A6:A37"/>
+    <sortCondition ref="C6:C37"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:A13">
+  <conditionalFormatting sqref="A6:A14">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
@@ -8251,9 +8520,9 @@
       <formula>6043</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B13" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
-      <formula1>$A$1048554:$A$1048560</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B37" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+      <formula1>$A$1048552:$A$1048558</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
U 1Q - Cuatrimestre 2023 (28032023)
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A286FF0-0DA2-492C-B117-7F2530741E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1FB36-6B9B-4ECC-A45B-921DE9D2A782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="178">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -544,6 +544,54 @@
   </si>
   <si>
     <t>OBS</t>
+  </si>
+  <si>
+    <t>wsalguero@gmail.com</t>
+  </si>
+  <si>
+    <t>gerardo.gonzaleztulian@gmail.com</t>
+  </si>
+  <si>
+    <t>jmatteucci@gmail.com</t>
+  </si>
+  <si>
+    <t>marina.surace@docentes.unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>nachocastillo@hotmail.com</t>
+  </si>
+  <si>
+    <t>cristianciarallo@gmail.com</t>
+  </si>
+  <si>
+    <t>jorge.insfran@gmail.com</t>
+  </si>
+  <si>
+    <t>dafernandez@gmail.com</t>
+  </si>
+  <si>
+    <t>leandro.cosentino@docentes.unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>zavhier@gmail.com</t>
+  </si>
+  <si>
+    <t>tlatorre@unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>olmos_azul@hotmail.com</t>
+  </si>
+  <si>
+    <t>fabyfep67@gmail.com</t>
+  </si>
+  <si>
+    <t>jefunesc@gmail.com</t>
+  </si>
+  <si>
+    <t>FUNES JUAN</t>
+  </si>
+  <si>
+    <t>ernesto.aguaysol@docentes.unpaz.edu.ar</t>
   </si>
 </sst>
 </file>
@@ -557,7 +605,7 @@
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,6 +725,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -737,7 +793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -751,8 +807,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -823,6 +880,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,10 +907,8 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Comma" xfId="5" xr:uid="{05F99610-EFDD-41FA-9067-2D9EACE38C58}"/>
     <cellStyle name="Comma [0]" xfId="6" xr:uid="{831A5D17-50A8-436C-BB84-397C03B818B8}"/>
     <cellStyle name="Currency" xfId="3" xr:uid="{BF8142CC-1AF6-420D-B027-00099720A01F}"/>
@@ -855,6 +916,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" hidden="1" xr:uid="{8E04FE8C-2ABB-4212-BBE6-EDA0B58F4578}"/>
     <cellStyle name="Followed Hyperlink" xfId="9" hidden="1" xr:uid="{3F7788B8-0DD1-40BF-84EB-FA451DE21CBE}"/>
     <cellStyle name="Followed Hyperlink" xfId="10" hidden="1" xr:uid="{58767AE6-8E09-46A2-8DA4-D5413B3C5FB6}"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="7" hidden="1" xr:uid="{D532F779-8519-4208-BEB3-555EF0129069}"/>
     <cellStyle name="Hyperlink" xfId="12" xr:uid="{60D493E0-0A33-4A4B-A94E-4B6753ECFD91}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4841,10 +4903,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="13">
         <f>GETPIVOTDATA("FULLNAME",$A$4)</f>
         <v>43</v>
@@ -5262,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5272,7 +5334,7 @@
     <col min="2" max="2" width="42.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1"/>
+    <col min="5" max="5" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" style="2" customWidth="1"/>
@@ -5283,42 +5345,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
@@ -5368,7 +5430,9 @@
       <c r="D5" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="32" t="s">
+        <v>173</v>
+      </c>
       <c r="F5" s="9">
         <f>VLOOKUP(A5,DEPIT!A4:J43,7,0)</f>
         <v>44382</v>
@@ -5383,7 +5447,7 @@
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5407,7 +5471,9 @@
       <c r="D6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="F6" s="9">
         <f>VLOOKUP(A6,DEPIT!A5:J44,7,0)</f>
         <v>44165</v>
@@ -5422,7 +5488,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5446,7 +5512,9 @@
       <c r="D7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="32" t="s">
+        <v>166</v>
+      </c>
       <c r="F7" s="9">
         <f>VLOOKUP(A7,DEPIT!A6:J45,7,0)</f>
         <v>44165</v>
@@ -5461,7 +5529,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5485,7 +5553,9 @@
       <c r="D8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="32" t="s">
+        <v>164</v>
+      </c>
       <c r="F8" s="9">
         <f>VLOOKUP(A8,DEPIT!A7:J46,7,0)</f>
         <v>0</v>
@@ -5500,7 +5570,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5524,7 +5594,9 @@
       <c r="D9" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="F9" s="9">
         <f>VLOOKUP(A9,DEPIT!A8:J47,7,0)</f>
         <v>44165</v>
@@ -5539,7 +5611,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5563,7 +5635,9 @@
       <c r="D10" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="32" t="s">
+        <v>173</v>
+      </c>
       <c r="F10" s="9">
         <f>VLOOKUP(A10,DEPIT!A8:J49,7,0)</f>
         <v>44512</v>
@@ -5578,7 +5652,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5602,7 +5676,9 @@
       <c r="D11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="32" t="s">
+        <v>173</v>
+      </c>
       <c r="F11" s="9">
         <f>VLOOKUP(A11,DEPIT!A8:J50,7,0)</f>
         <v>44512</v>
@@ -5617,7 +5693,7 @@
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5641,7 +5717,9 @@
       <c r="D12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="32" t="s">
+        <v>166</v>
+      </c>
       <c r="F12" s="9">
         <f>VLOOKUP(A12,DEPIT!A9:J51,7,0)</f>
         <v>44512</v>
@@ -5656,7 +5734,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5680,7 +5758,9 @@
       <c r="D13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="F13" s="9">
         <f>VLOOKUP(A13,DEPIT!A10:J52,7,0)</f>
         <v>44165</v>
@@ -5695,7 +5775,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5719,7 +5799,9 @@
       <c r="D14" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="32" t="s">
+        <v>165</v>
+      </c>
       <c r="F14" s="9">
         <f>VLOOKUP(A14,DEPIT!A11:J53,7,0)</f>
         <v>44512</v>
@@ -5734,7 +5816,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5758,7 +5840,9 @@
       <c r="D15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="F15" s="9">
         <f>VLOOKUP(A15,DEPIT!A12:J54,7,0)</f>
         <v>44165</v>
@@ -5773,7 +5857,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5810,7 +5894,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5834,7 +5918,9 @@
       <c r="D17" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="32" t="s">
+        <v>165</v>
+      </c>
       <c r="F17" s="9">
         <f>VLOOKUP(A17,DEPIT!A14:J56,7,0)</f>
         <v>44165</v>
@@ -5849,7 +5935,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5870,8 +5956,12 @@
       <c r="C18" s="8">
         <v>2</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="F18" s="9">
         <f>VLOOKUP(A18,DEPIT!A15:J57,7,0)</f>
         <v>0</v>
@@ -5886,7 +5976,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5910,7 +6000,9 @@
       <c r="D19" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="32" t="s">
+        <v>163</v>
+      </c>
       <c r="F19" s="9">
         <f>VLOOKUP(A19,DEPIT!A16:J58,7,0)</f>
         <v>0</v>
@@ -5925,7 +6017,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5949,7 +6041,9 @@
       <c r="D20" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="32" t="s">
+        <v>174</v>
+      </c>
       <c r="F20" s="9">
         <f>VLOOKUP(A20,DEPIT!A17:J59,7,0)</f>
         <v>44705</v>
@@ -5964,7 +6058,7 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5988,7 +6082,9 @@
       <c r="D21" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="32" t="s">
+        <v>163</v>
+      </c>
       <c r="F21" s="9">
         <f>VLOOKUP(A21,DEPIT!A18:J60,7,0)</f>
         <v>0</v>
@@ -6003,7 +6099,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6027,7 +6123,9 @@
       <c r="D22" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="32" t="s">
+        <v>167</v>
+      </c>
       <c r="F22" s="9">
         <f>VLOOKUP(A22,DEPIT!A19:J61,7,0)</f>
         <v>0</v>
@@ -6042,7 +6140,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6066,7 +6164,9 @@
       <c r="D23" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="32" t="s">
+        <v>168</v>
+      </c>
       <c r="F23" s="9">
         <f>VLOOKUP(A23,DEPIT!A20:J62,7,0)</f>
         <v>44697</v>
@@ -6081,7 +6181,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6118,7 +6218,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6155,7 +6255,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6176,8 +6276,12 @@
       <c r="C26" s="8">
         <v>3</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>175</v>
+      </c>
       <c r="F26" s="9">
         <f>VLOOKUP(A26,DEPIT!A23:J65,7,0)</f>
         <v>44512</v>
@@ -6192,7 +6296,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6229,7 +6333,7 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6266,7 +6370,7 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6290,7 +6394,9 @@
       <c r="D29" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="32" t="s">
+        <v>169</v>
+      </c>
       <c r="F29" s="9">
         <f>VLOOKUP(A29,DEPIT!A26:J68,7,0)</f>
         <v>44512</v>
@@ -6305,7 +6411,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6329,7 +6435,9 @@
       <c r="D30" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="32" t="s">
+        <v>172</v>
+      </c>
       <c r="F30" s="9">
         <f>VLOOKUP(A30,DEPIT!A27:J69,7,0)</f>
         <v>0</v>
@@ -6344,7 +6452,7 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6381,7 +6489,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6405,7 +6513,9 @@
       <c r="D32" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="32" t="s">
+        <v>163</v>
+      </c>
       <c r="F32" s="9">
         <f>VLOOKUP(A32,DEPIT!A29:J71,7,0)</f>
         <v>0</v>
@@ -6420,7 +6530,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6457,7 +6567,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6494,7 +6604,7 @@
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6531,7 +6641,7 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-141</v>
+        <v>-153</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6568,7 +6678,7 @@
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6605,7 +6715,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6629,7 +6739,9 @@
       <c r="D38" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="32" t="s">
+        <v>177</v>
+      </c>
       <c r="F38" s="9">
         <f>VLOOKUP(A38,DEPIT!A35:J77,7,0)</f>
         <v>0</v>
@@ -6644,7 +6756,7 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6668,7 +6780,9 @@
       <c r="D39" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="32" t="s">
+        <v>170</v>
+      </c>
       <c r="F39" s="9">
         <f>VLOOKUP(A39,DEPIT!A36:J78,7,0)</f>
         <v>0</v>
@@ -6683,7 +6797,7 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6720,7 +6834,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6757,7 +6871,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6781,7 +6895,9 @@
       <c r="D42" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E42" s="7"/>
+      <c r="E42" s="32" t="s">
+        <v>171</v>
+      </c>
       <c r="F42" s="9">
         <f>VLOOKUP(A42,DEPIT!A39:J81,7,0)</f>
         <v>0</v>
@@ -6796,7 +6912,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6833,7 +6949,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-106</v>
+        <v>-118</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6870,7 +6986,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6907,7 +7023,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6944,7 +7060,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6968,7 +7084,9 @@
       <c r="D47" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="32" t="s">
+        <v>169</v>
+      </c>
       <c r="F47" s="9">
         <f>VLOOKUP(A47,DEPIT!A44:J86,7,0)</f>
         <v>0</v>
@@ -6983,7 +7101,7 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44271</v>
+        <v>-44283</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6995,10 +7113,10 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="33"/>
+      <c r="B50" s="37"/>
     </row>
     <row r="51" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
@@ -7115,16 +7233,44 @@
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{416BB296-384D-4084-9F69-00515FE2086D}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{0DA617EF-AB3A-492A-9C35-87FC1313CB11}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{28F56E14-55DF-42DB-9C14-18653CA0D81B}"/>
+    <hyperlink ref="E15" r:id="rId4" xr:uid="{983E352A-3EA1-4BBD-954A-6AA4BD5D68AC}"/>
+    <hyperlink ref="E19" r:id="rId5" xr:uid="{69661847-D92B-40B0-8B65-5A03DCEAA2D9}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{BA72DE52-F32A-4152-B255-01F3EABDEA0E}"/>
+    <hyperlink ref="E14" r:id="rId7" xr:uid="{198F0087-308D-4015-B943-C30E2EBCAB13}"/>
+    <hyperlink ref="E17" r:id="rId8" xr:uid="{0D8FEB1A-44F8-4116-AD78-8EFFA92B1C3B}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{4519BE65-C749-44F1-8F40-7E2DCEB88562}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{44F48037-19F9-47F5-9F26-999E0115289A}"/>
+    <hyperlink ref="E21" r:id="rId11" xr:uid="{96F313D5-BD45-4B6A-A517-BB99414B9271}"/>
+    <hyperlink ref="E22" r:id="rId12" xr:uid="{D13FE835-CD25-43EB-A603-64F468606E2C}"/>
+    <hyperlink ref="E23" r:id="rId13" xr:uid="{2CDA0495-C49E-40A9-81E1-21B16746F504}"/>
+    <hyperlink ref="E29" r:id="rId14" xr:uid="{97066505-D123-4941-BF10-D9A2FE038432}"/>
+    <hyperlink ref="E47" r:id="rId15" xr:uid="{46A73F4D-F596-4F3D-BEF9-DB7538AE1F62}"/>
+    <hyperlink ref="E32" r:id="rId16" xr:uid="{655E35C1-1FDC-4B53-AC61-AEFF20AAF575}"/>
+    <hyperlink ref="E39" r:id="rId17" xr:uid="{E465FA0A-0341-453D-A1D3-88AF00DEC21E}"/>
+    <hyperlink ref="E42" r:id="rId18" xr:uid="{429019C6-2A42-4AC9-A725-D0E3A01EF864}"/>
+    <hyperlink ref="E30" r:id="rId19" xr:uid="{B5F191CC-86CF-4A0E-B25B-2343C541DC9E}"/>
+    <hyperlink ref="E5" r:id="rId20" xr:uid="{091CBF36-24D9-404F-9E33-1B33AFF26A8F}"/>
+    <hyperlink ref="E10" r:id="rId21" xr:uid="{4B9A1D75-A314-4557-B542-F1B822529F84}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{18E767FD-E0B0-4F20-9964-A5D9EB7B7DA1}"/>
+    <hyperlink ref="E18" r:id="rId23" xr:uid="{806C0922-CB76-4E42-9FFA-287F729BF6D4}"/>
+    <hyperlink ref="E20" r:id="rId24" xr:uid="{3EB28842-B6B1-4575-80F2-3D1A2C7BCDC4}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{BF68D9C3-B8D7-4711-9592-9E15A45F931E}"/>
+    <hyperlink ref="E38" r:id="rId26" xr:uid="{259744C5-F7C2-499C-9771-C82AF29773EE}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId27"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;CUniversidad Nacional de José C. Paz (UNPAZ)
 </oddHeader>
     <oddFooter>&amp;CDepartamento de Economía, Producción E Innovación Tecnológica&amp;R&amp;D</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7157,22 +7303,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
@@ -8041,8 +8187,8 @@
   </sheetPr>
   <dimension ref="A2:G1048558"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8055,26 +8201,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
@@ -8097,7 +8243,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="37">
+      <c r="A6" s="30">
         <v>6002</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -8109,20 +8255,22 @@
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="37">
+      <c r="A7" s="30">
+        <v>6002</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45005</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="30">
         <v>6003</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="37">
-        <v>6004</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>150</v>
@@ -8130,25 +8278,24 @@
       <c r="C8" s="9">
         <v>45000</v>
       </c>
-      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="37">
-        <v>6004</v>
+      <c r="A9" s="30">
+        <v>6003</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C9" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D9" s="8" t="s">
+        <v>45012</v>
+      </c>
+      <c r="D9" s="33" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="37">
-        <v>6005</v>
+      <c r="A10" s="30">
+        <v>6004</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>150</v>
@@ -8159,20 +8306,22 @@
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="37">
-        <v>6009</v>
+      <c r="A11" s="30">
+        <v>6004</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D11" s="8"/>
+        <v>45001</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="37">
-        <v>6011</v>
+      <c r="A12" s="30">
+        <v>6005</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>150</v>
@@ -8183,19 +8332,22 @@
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="38">
-        <v>6012</v>
+      <c r="A13" s="30">
+        <v>6005</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C13" s="9">
-        <v>45001</v>
+        <v>45005</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="37">
-        <v>6013</v>
+      <c r="A14" s="30">
+        <v>6009</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>150</v>
@@ -8206,45 +8358,48 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="38">
-        <v>6014</v>
+      <c r="A15" s="30">
+        <v>6009</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C15" s="9">
-        <v>45001</v>
+        <v>45005</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="38">
-        <v>6015</v>
+      <c r="A16" s="30">
+        <v>6011</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C16" s="9">
-        <v>45001</v>
+        <v>45000</v>
       </c>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="38">
-        <v>6015</v>
+      <c r="A17" s="30">
+        <v>6011</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C17" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D17" s="8" t="s">
+        <v>45005</v>
+      </c>
+      <c r="D17" s="33" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="38">
-        <v>6017</v>
+      <c r="A18" s="31">
+        <v>6012</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>150</v>
@@ -8254,19 +8409,20 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="38">
-        <v>6018</v>
+      <c r="A19" s="30">
+        <v>6013</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C19" s="9">
-        <v>45001</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="38">
-        <v>6020</v>
+      <c r="A20" s="31">
+        <v>6014</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>150</v>
@@ -8276,8 +8432,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="38">
-        <v>6024</v>
+      <c r="A21" s="31">
+        <v>6015</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>150</v>
@@ -8285,21 +8441,25 @@
       <c r="C21" s="9">
         <v>45001</v>
       </c>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="38">
-        <v>6026</v>
+      <c r="A22" s="31">
+        <v>6015</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C22" s="9">
         <v>45001</v>
       </c>
+      <c r="D22" s="33" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="38">
-        <v>6027</v>
+      <c r="A23" s="31">
+        <v>6017</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>150</v>
@@ -8309,8 +8469,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="38">
-        <v>6028</v>
+      <c r="A24" s="31">
+        <v>6018</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>150</v>
@@ -8320,8 +8480,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="38">
-        <v>6029</v>
+      <c r="A25" s="31">
+        <v>6020</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>150</v>
@@ -8331,20 +8491,19 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="37">
-        <v>6031</v>
+      <c r="A26" s="31">
+        <v>6024</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C26" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D26" s="8"/>
+        <v>45001</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="38">
-        <v>6032</v>
+      <c r="A27" s="31">
+        <v>6026</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>150</v>
@@ -8354,8 +8513,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="38">
-        <v>6033</v>
+      <c r="A28" s="31">
+        <v>6027</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>150</v>
@@ -8365,8 +8524,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="38">
-        <v>6034</v>
+      <c r="A29" s="31">
+        <v>6028</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>150</v>
@@ -8376,8 +8535,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="38">
-        <v>6035</v>
+      <c r="A30" s="31">
+        <v>6029</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>150</v>
@@ -8387,30 +8546,34 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="38">
-        <v>6036</v>
+      <c r="A31" s="30">
+        <v>6031</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C31" s="9">
-        <v>45001</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="38">
-        <v>6037</v>
+      <c r="A32" s="30">
+        <v>6031</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C32" s="9">
-        <v>45001</v>
+        <v>45013</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A33" s="38">
-        <v>6038</v>
+      <c r="A33" s="31">
+        <v>6032</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>150</v>
@@ -8420,8 +8583,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A34" s="38">
-        <v>6040</v>
+      <c r="A34" s="31">
+        <v>6033</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>150</v>
@@ -8431,8 +8594,8 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" s="38">
-        <v>6041</v>
+      <c r="A35" s="31">
+        <v>6034</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>150</v>
@@ -8442,8 +8605,8 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="38">
-        <v>6042</v>
+      <c r="A36" s="31">
+        <v>6035</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>150</v>
@@ -8453,13 +8616,79 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A37" s="38">
-        <v>6043</v>
+      <c r="A37" s="31">
+        <v>6036</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C37" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" s="31">
+        <v>6037</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C38" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" s="31">
+        <v>6038</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" s="31">
+        <v>6040</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" s="31">
+        <v>6041</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" s="31">
+        <v>6042</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" s="31">
+        <v>6043</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="9">
         <v>45001</v>
       </c>
     </row>
@@ -8504,15 +8733,15 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F37">
-    <sortCondition ref="A6:A37"/>
-    <sortCondition ref="C6:C37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F43">
+    <sortCondition ref="A6:A43"/>
+    <sortCondition ref="C6:C43"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:A14">
+  <conditionalFormatting sqref="A6:A15">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
@@ -8521,11 +8750,21 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B37" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B43" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
       <formula1>$A$1048552:$A$1048558</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" tooltip="6004" xr:uid="{98815502-696A-4ED7-8F42-1713E48F3EEC}"/>
+    <hyperlink ref="D17" r:id="rId2" tooltip="6011" xr:uid="{24D0A05B-C8EE-4787-96DB-2A89DF2B0D89}"/>
+    <hyperlink ref="D7" r:id="rId3" tooltip="6002" xr:uid="{214F1D65-92A0-4C91-848F-31097B9C11FD}"/>
+    <hyperlink ref="D13" r:id="rId4" tooltip="6005" xr:uid="{C3CBAD01-E9C1-49F4-A848-4C351A0AC29A}"/>
+    <hyperlink ref="D15" r:id="rId5" tooltip="6009" xr:uid="{41977E1C-88AC-44D4-B0F8-0341DA06AB2C}"/>
+    <hyperlink ref="D22" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
+    <hyperlink ref="D9" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
+    <hyperlink ref="D32" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de UUCC – LGTI Q1A2023E01
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F1FB36-6B9B-4ECC-A45B-921DE9D2A782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADA3193-CEC2-4C27-BE29-5B3C95DB0181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLERO" sheetId="5" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="178">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -942,192 +942,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1489,6 +1303,192 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4518,29 +4518,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="19">
       <calculatedColumnFormula>VLOOKUP(A5,DEPIT!A4:J43,7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="36">
+    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="18">
       <calculatedColumnFormula>F5+(365*2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="35">
+    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="17">
       <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="16">
       <calculatedColumnFormula>G5 - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="33">
+    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="15">
       <calculatedColumnFormula>IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="32">
+    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="14">
       <calculatedColumnFormula>CONCATENATE(Tabla7[[#This Row],[CÓDIGO]]," - ",Tabla7[[#This Row],[ASIGNATURA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4549,23 +4549,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A4:J49" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J49">
     <sortCondition ref="A5:A49"/>
     <sortCondition descending="1" ref="G5:G49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5324,8 +5324,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5529,7 +5529,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5611,7 +5611,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5816,7 +5816,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6058,7 +6058,7 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6140,7 +6140,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6181,7 +6181,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6255,7 +6255,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6296,7 +6296,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6333,7 +6333,7 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6370,7 +6370,7 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6411,7 +6411,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6452,7 +6452,7 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6489,7 +6489,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6530,7 +6530,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6604,7 +6604,7 @@
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-153</v>
+        <v>-154</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6715,7 +6715,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6871,7 +6871,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6949,7 +6949,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-118</v>
+        <v>-119</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7060,7 +7060,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44283</v>
+        <v>-44284</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7152,84 +7152,84 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I5:I47">
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="25" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="21" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H47">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1901">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="1901">
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8187,8 +8187,8 @@
   </sheetPr>
   <dimension ref="A2:G1048558"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8571,7 +8571,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="31">
         <v>6032</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="31">
         <v>6033</v>
       </c>
@@ -8593,7 +8593,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="31">
         <v>6034</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" s="31">
         <v>6035</v>
       </c>
@@ -8615,20 +8615,23 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" s="31">
+        <v>6035</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="9">
+        <v>45013</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="31">
         <v>6036</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A38" s="31">
-        <v>6037</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>150</v>
@@ -8637,9 +8640,9 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="31">
-        <v>6038</v>
+        <v>6037</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>150</v>
@@ -8648,9 +8651,9 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="31">
-        <v>6040</v>
+        <v>6038</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>150</v>
@@ -8659,9 +8662,9 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" s="31">
-        <v>6041</v>
+        <v>6040</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>150</v>
@@ -8670,9 +8673,9 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" s="31">
-        <v>6042</v>
+        <v>6041</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>150</v>
@@ -8681,14 +8684,25 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="31">
-        <v>6043</v>
+        <v>6042</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C43" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" s="31">
+        <v>6043</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="9">
         <v>45001</v>
       </c>
     </row>
@@ -8733,9 +8747,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F43">
-    <sortCondition ref="A6:A43"/>
-    <sortCondition ref="C6:C43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F44">
+    <sortCondition ref="A6:A44"/>
+    <sortCondition ref="C6:C44"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
@@ -8750,7 +8764,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B43" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B44" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
       <formula1>$A$1048552:$A$1048558</formula1>
     </dataValidation>
   </dataValidations>
@@ -8763,8 +8777,9 @@
     <hyperlink ref="D22" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
     <hyperlink ref="D9" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
     <hyperlink ref="D32" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
+    <hyperlink ref="D37" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de UUCC – LGTI Q1A2023E02
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADA3193-CEC2-4C27-BE29-5B3C95DB0181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F062AA29-BD14-47F9-9AA3-6BA32EF0D733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLERO" sheetId="5" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -592,6 +592,18 @@
   </si>
   <si>
     <t>ernesto.aguaysol@docentes.unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>JAVIER BILATZ</t>
+  </si>
+  <si>
+    <t>javier.bilatz@docentes.unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>storres@unpaz.edu.ar</t>
+  </si>
+  <si>
+    <t>SERGIO TORRES</t>
   </si>
 </sst>
 </file>
@@ -1527,6 +1539,14 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <name val="Segoe UI"/>
         <scheme val="none"/>
@@ -1554,14 +1574,6 @@
       <font>
         <name val="Segoe UI"/>
         <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
       </font>
     </dxf>
   </dxfs>
@@ -4001,168 +4013,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1534DF67-168C-48EE-A5F4-F1BC3F91C55C}" name="TablaDinámica33" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
-  <location ref="D10:E13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="3">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-      </items>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Total" fld="0" subtotal="count" baseField="8" baseItem="0"/>
-  </dataFields>
-  <formats count="5">
-    <format dxfId="49">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="48">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="47">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09B2CF50-50DC-4CF0-A0B1-303344D40A0A}" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A4:B48" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
@@ -4428,36 +4278,36 @@
     <dataField name="#" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="57">
+    <format dxfId="52">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="50">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="49">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="48">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4465,6 +4315,168 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1534DF67-168C-48EE-A5F4-F1BC3F91C55C}" name="TablaDinámica33" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
+  <location ref="D10:E13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="3">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total" fld="0" subtotal="count" baseField="8" baseItem="0"/>
+  </dataFields>
+  <formats count="5">
+    <format dxfId="57">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="56">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="55">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="54">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="53">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
       <xpdl:pivotTableDefinition16/>
@@ -5324,8 +5336,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:B39"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5447,7 +5459,7 @@
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5488,7 +5500,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5529,7 +5541,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5570,7 +5582,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5611,7 +5623,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5652,7 +5664,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5693,7 +5705,7 @@
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5734,7 +5746,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5775,7 +5787,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5816,7 +5828,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5857,7 +5869,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5894,7 +5906,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5935,7 +5947,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5976,7 +5988,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6017,7 +6029,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6058,7 +6070,7 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6099,7 +6111,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6140,7 +6152,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6181,7 +6193,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6218,7 +6230,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6255,7 +6267,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6296,7 +6308,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6333,7 +6345,7 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6370,7 +6382,7 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6411,7 +6423,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6452,7 +6464,7 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6489,7 +6501,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6530,7 +6542,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6567,7 +6579,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6588,8 +6600,12 @@
       <c r="C34" s="8">
         <v>4</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="D34" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>179</v>
+      </c>
       <c r="F34" s="9">
         <f>VLOOKUP(A34,DEPIT!A31:J73,7,0)</f>
         <v>44512</v>
@@ -6604,7 +6620,7 @@
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6625,8 +6641,12 @@
       <c r="C35" s="8">
         <v>4</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
+      <c r="D35" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>180</v>
+      </c>
       <c r="F35" s="9">
         <f>VLOOKUP(A35,DEPIT!A32:J74,7,0)</f>
         <v>44130</v>
@@ -6641,7 +6661,7 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-154</v>
+        <v>-159</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6678,7 +6698,7 @@
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6715,7 +6735,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6756,7 +6776,7 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6797,7 +6817,7 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6834,7 +6854,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6871,7 +6891,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6912,7 +6932,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6933,8 +6953,12 @@
       <c r="C43" s="8">
         <v>5</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
+      <c r="D43" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>168</v>
+      </c>
       <c r="F43" s="9">
         <f>VLOOKUP(A43,DEPIT!A40:J82,7,0)</f>
         <v>44165</v>
@@ -6949,7 +6973,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-119</v>
+        <v>-124</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6986,7 +7010,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7023,7 +7047,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7060,7 +7084,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7101,7 +7125,7 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44284</v>
+        <v>-44289</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7260,17 +7284,19 @@
     <hyperlink ref="E20" r:id="rId24" xr:uid="{3EB28842-B6B1-4575-80F2-3D1A2C7BCDC4}"/>
     <hyperlink ref="E26" r:id="rId25" xr:uid="{BF68D9C3-B8D7-4711-9592-9E15A45F931E}"/>
     <hyperlink ref="E38" r:id="rId26" xr:uid="{259744C5-F7C2-499C-9771-C82AF29773EE}"/>
+    <hyperlink ref="E43" r:id="rId27" xr:uid="{D89BD6D8-127E-49D6-8D91-D61D3301D412}"/>
+    <hyperlink ref="E34" r:id="rId28" xr:uid="{8AC348C1-0792-4A63-B15A-949010A3C799}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="landscape" r:id="rId27"/>
+  <pageSetup orientation="landscape" r:id="rId29"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;CUniversidad Nacional de José C. Paz (UNPAZ)
 </oddHeader>
     <oddFooter>&amp;CDepartamento de Economía, Producción E Innovación Tecnológica&amp;R&amp;D</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8187,7 +8213,7 @@
   </sheetPr>
   <dimension ref="A2:G1048558"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Envio de UUCC – LGTI Q1A2023E03
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F062AA29-BD14-47F9-9AA3-6BA32EF0D733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFDBB33-5D5C-439D-AE72-B17D404FFF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="182">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -936,7 +936,7 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{561F4419-9779-48EA-98E4-826F7DD662D5}"/>
     <cellStyle name="Percent" xfId="2" xr:uid="{CDE64AD3-5503-4CAE-82E9-E24CD1038088}"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="60">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -954,6 +954,212 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1315,192 +1521,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4278,36 +4298,36 @@
     <dataField name="#" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="52">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="51">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="52">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="51">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="50">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4424,23 +4444,23 @@
     <dataField name="Total" fld="0" subtotal="count" baseField="8" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="57">
+    <format dxfId="59">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="58">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="57">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4530,29 +4550,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="39">
       <calculatedColumnFormula>VLOOKUP(A5,DEPIT!A4:J43,7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="38">
       <calculatedColumnFormula>F5+(365*2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="37">
       <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="16">
+    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="36">
       <calculatedColumnFormula>G5 - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="35">
       <calculatedColumnFormula>IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="14">
+    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="34">
       <calculatedColumnFormula>CONCATENATE(Tabla7[[#This Row],[CÓDIGO]]," - ",Tabla7[[#This Row],[ASIGNATURA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4561,23 +4581,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A4:J49" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J49">
     <sortCondition ref="A5:A49"/>
     <sortCondition descending="1" ref="G5:G49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5459,7 +5479,7 @@
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5500,7 +5520,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5541,7 +5561,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5582,7 +5602,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5623,7 +5643,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5664,7 +5684,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5705,7 +5725,7 @@
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5746,7 +5766,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5787,7 +5807,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5828,7 +5848,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5869,7 +5889,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5906,7 +5926,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5947,7 +5967,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5988,7 +6008,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6029,7 +6049,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6070,7 +6090,7 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6111,7 +6131,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6152,7 +6172,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6193,7 +6213,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6230,7 +6250,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6267,7 +6287,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6308,7 +6328,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6345,7 +6365,7 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6382,7 +6402,7 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6423,7 +6443,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6464,7 +6484,7 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6501,7 +6521,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6542,7 +6562,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6579,7 +6599,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6620,7 +6640,7 @@
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6661,7 +6681,7 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-159</v>
+        <v>-160</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6698,7 +6718,7 @@
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6735,7 +6755,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6776,7 +6796,7 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6817,7 +6837,7 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6854,7 +6874,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6891,7 +6911,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6932,7 +6952,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6973,7 +6993,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-124</v>
+        <v>-125</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7010,7 +7030,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7047,7 +7067,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7084,7 +7104,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7125,7 +7145,7 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44289</v>
+        <v>-44290</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7176,84 +7196,84 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I5:I47">
-    <cfRule type="cellIs" dxfId="44" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="42" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H47">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="1901">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="1901">
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8211,10 +8231,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A2:G1048558"/>
+  <dimension ref="A2:G1048559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8665,6 +8685,7 @@
       <c r="C38" s="9">
         <v>45001</v>
       </c>
+      <c r="D38" s="33"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" s="31">
@@ -8676,6 +8697,7 @@
       <c r="C39" s="9">
         <v>45001</v>
       </c>
+      <c r="D39" s="33"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" s="31">
@@ -8687,32 +8709,37 @@
       <c r="C40" s="9">
         <v>45001</v>
       </c>
+      <c r="D40" s="33"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" s="31">
-        <v>6040</v>
+      <c r="A41" s="30">
+        <v>6039</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="9">
-        <v>45001</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="31">
-        <v>6041</v>
+      <c r="A42" s="30">
+        <v>6039</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C42" s="9">
-        <v>45001</v>
+        <v>45020</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" s="31">
-        <v>6042</v>
+        <v>6040</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>150</v>
@@ -8720,10 +8747,11 @@
       <c r="C43" s="9">
         <v>45001</v>
       </c>
+      <c r="D43" s="33"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" s="31">
-        <v>6043</v>
+        <v>6041</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>150</v>
@@ -8731,57 +8759,90 @@
       <c r="C44" s="9">
         <v>45001</v>
       </c>
-    </row>
-    <row r="1048551" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048551" s="7" t="s">
+      <c r="D44" s="33"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" s="31">
+        <v>6042</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D45" s="33"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" s="31">
+        <v>6043</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D46" s="33"/>
+    </row>
+    <row r="1048552" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048552" s="7" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="1048552" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048552" s="29" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="1048553" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048553" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="1048554" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048554" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="1048555" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048555" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="1048556" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048556" s="29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="1048557" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048557" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="1048558" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048558" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1048559" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048559" s="29" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F44">
-    <sortCondition ref="A6:A44"/>
-    <sortCondition ref="C6:C44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F46">
+    <sortCondition ref="A6:A46"/>
+    <sortCondition ref="C6:C46"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:A15">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>6001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>6043</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:A42">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
@@ -8790,8 +8851,8 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B44" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
-      <formula1>$A$1048552:$A$1048558</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B46" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+      <formula1>$A$1048553:$A$1048559</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -8804,8 +8865,9 @@
     <hyperlink ref="D9" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
     <hyperlink ref="D32" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
     <hyperlink ref="D37" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
+    <hyperlink ref="D42" r:id="rId10" tooltip="6039" xr:uid="{5CFF6145-29E8-4D14-91C2-F8073B207DDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de UUCC – LGTI Q1A2023E04
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\01.UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFDBB33-5D5C-439D-AE72-B17D404FFF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B75A83-E1A8-4783-8200-D60079B19D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="188">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -516,15 +516,6 @@
     <t>Recepción del profesor</t>
   </si>
   <si>
-    <t>Envió Desarrollo curricular</t>
-  </si>
-  <si>
-    <t>Ajustes Desarrollo curricular</t>
-  </si>
-  <si>
-    <t>Aprobado Desarrollo curricular</t>
-  </si>
-  <si>
     <t>Envío DEPIT</t>
   </si>
   <si>
@@ -604,6 +595,33 @@
   </si>
   <si>
     <t>SERGIO TORRES</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC  | 6002-6005-6009-6011</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC | 6003</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC | 6015</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC | 6031</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC | 6035</t>
+  </si>
+  <si>
+    <t>Ajustes UUCC | 6039</t>
+  </si>
+  <si>
+    <t>Envío a Desarrollo curricular</t>
+  </si>
+  <si>
+    <t>Rectificada / Aprobada</t>
+  </si>
+  <si>
+    <t>En Modificación</t>
   </si>
 </sst>
 </file>
@@ -746,7 +764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,18 +801,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -821,7 +827,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -892,8 +898,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="13" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -919,6 +923,7 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma" xfId="5" xr:uid="{05F99610-EFDD-41FA-9067-2D9EACE38C58}"/>
@@ -936,7 +941,267 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{561F4419-9779-48EA-98E4-826F7DD662D5}"/>
     <cellStyle name="Percent" xfId="2" xr:uid="{CDE64AD3-5503-4CAE-82E9-E24CD1038088}"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="86">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4298,36 +4563,36 @@
     <dataField name="#" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="54">
+    <format dxfId="80">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="78">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="77">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="76">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="75">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4444,23 +4709,23 @@
     <dataField name="Total" fld="0" subtotal="count" baseField="8" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="59">
+    <format dxfId="85">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="58">
+    <format dxfId="84">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="83">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4550,29 +4815,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="65">
       <calculatedColumnFormula>VLOOKUP(A5,DEPIT!A4:J43,7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="38">
+    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="64">
       <calculatedColumnFormula>F5+(365*2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="37">
+    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="63">
       <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="36">
+    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="62">
       <calculatedColumnFormula>G5 - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="35">
+    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="61">
       <calculatedColumnFormula>IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="34">
+    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="60">
       <calculatedColumnFormula>CONCATENATE(Tabla7[[#This Row],[CÓDIGO]]," - ",Tabla7[[#This Row],[ASIGNATURA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4581,23 +4846,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A4:J49" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J49">
     <sortCondition ref="A5:A49"/>
     <sortCondition descending="1" ref="G5:G49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="49"/>
+    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4935,10 +5200,10 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="34"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="13">
         <f>GETPIVOTDATA("FULLNAME",$A$4)</f>
         <v>43</v>
@@ -5377,42 +5642,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="16" t="s">
@@ -5462,8 +5727,8 @@
       <c r="D5" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>173</v>
+      <c r="E5" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="F5" s="9">
         <f>VLOOKUP(A5,DEPIT!A4:J43,7,0)</f>
@@ -5479,7 +5744,7 @@
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5503,8 +5768,8 @@
       <c r="D6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>162</v>
+      <c r="E6" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F6" s="9">
         <f>VLOOKUP(A6,DEPIT!A5:J44,7,0)</f>
@@ -5520,7 +5785,7 @@
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5544,8 +5809,8 @@
       <c r="D7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>166</v>
+      <c r="E7" s="30" t="s">
+        <v>163</v>
       </c>
       <c r="F7" s="9">
         <f>VLOOKUP(A7,DEPIT!A6:J45,7,0)</f>
@@ -5561,7 +5826,7 @@
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5585,8 +5850,8 @@
       <c r="D8" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>164</v>
+      <c r="E8" s="30" t="s">
+        <v>161</v>
       </c>
       <c r="F8" s="9">
         <f>VLOOKUP(A8,DEPIT!A7:J46,7,0)</f>
@@ -5602,7 +5867,7 @@
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5626,8 +5891,8 @@
       <c r="D9" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>162</v>
+      <c r="E9" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F9" s="9">
         <f>VLOOKUP(A9,DEPIT!A8:J47,7,0)</f>
@@ -5643,7 +5908,7 @@
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5667,8 +5932,8 @@
       <c r="D10" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>173</v>
+      <c r="E10" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="F10" s="9">
         <f>VLOOKUP(A10,DEPIT!A8:J49,7,0)</f>
@@ -5684,7 +5949,7 @@
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5708,8 +5973,8 @@
       <c r="D11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>173</v>
+      <c r="E11" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="F11" s="9">
         <f>VLOOKUP(A11,DEPIT!A8:J50,7,0)</f>
@@ -5725,7 +5990,7 @@
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5749,8 +6014,8 @@
       <c r="D12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E12" s="32" t="s">
-        <v>166</v>
+      <c r="E12" s="30" t="s">
+        <v>163</v>
       </c>
       <c r="F12" s="9">
         <f>VLOOKUP(A12,DEPIT!A9:J51,7,0)</f>
@@ -5766,7 +6031,7 @@
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5790,8 +6055,8 @@
       <c r="D13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="32" t="s">
-        <v>162</v>
+      <c r="E13" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F13" s="9">
         <f>VLOOKUP(A13,DEPIT!A10:J52,7,0)</f>
@@ -5807,7 +6072,7 @@
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5831,8 +6096,8 @@
       <c r="D14" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="32" t="s">
-        <v>165</v>
+      <c r="E14" s="30" t="s">
+        <v>162</v>
       </c>
       <c r="F14" s="9">
         <f>VLOOKUP(A14,DEPIT!A11:J53,7,0)</f>
@@ -5848,7 +6113,7 @@
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5872,8 +6137,8 @@
       <c r="D15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>162</v>
+      <c r="E15" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="F15" s="9">
         <f>VLOOKUP(A15,DEPIT!A12:J54,7,0)</f>
@@ -5889,7 +6154,7 @@
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5926,7 +6191,7 @@
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5950,8 +6215,8 @@
       <c r="D17" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>165</v>
+      <c r="E17" s="30" t="s">
+        <v>162</v>
       </c>
       <c r="F17" s="9">
         <f>VLOOKUP(A17,DEPIT!A14:J56,7,0)</f>
@@ -5967,7 +6232,7 @@
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5991,8 +6256,8 @@
       <c r="D18" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E18" s="32" t="s">
-        <v>171</v>
+      <c r="E18" s="30" t="s">
+        <v>168</v>
       </c>
       <c r="F18" s="9">
         <f>VLOOKUP(A18,DEPIT!A15:J57,7,0)</f>
@@ -6008,7 +6273,7 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6032,8 +6297,8 @@
       <c r="D19" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="32" t="s">
-        <v>163</v>
+      <c r="E19" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="F19" s="9">
         <f>VLOOKUP(A19,DEPIT!A16:J58,7,0)</f>
@@ -6049,7 +6314,7 @@
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6073,8 +6338,8 @@
       <c r="D20" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="32" t="s">
-        <v>174</v>
+      <c r="E20" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="F20" s="9">
         <f>VLOOKUP(A20,DEPIT!A17:J59,7,0)</f>
@@ -6090,7 +6355,7 @@
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6114,8 +6379,8 @@
       <c r="D21" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>163</v>
+      <c r="E21" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="F21" s="9">
         <f>VLOOKUP(A21,DEPIT!A18:J60,7,0)</f>
@@ -6131,7 +6396,7 @@
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6155,8 +6420,8 @@
       <c r="D22" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>167</v>
+      <c r="E22" s="30" t="s">
+        <v>164</v>
       </c>
       <c r="F22" s="9">
         <f>VLOOKUP(A22,DEPIT!A19:J61,7,0)</f>
@@ -6172,7 +6437,7 @@
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6196,8 +6461,8 @@
       <c r="D23" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="32" t="s">
-        <v>168</v>
+      <c r="E23" s="30" t="s">
+        <v>165</v>
       </c>
       <c r="F23" s="9">
         <f>VLOOKUP(A23,DEPIT!A20:J62,7,0)</f>
@@ -6213,7 +6478,7 @@
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6250,7 +6515,7 @@
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6287,7 +6552,7 @@
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6309,10 +6574,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="F26" s="9">
         <f>VLOOKUP(A26,DEPIT!A23:J65,7,0)</f>
@@ -6328,7 +6593,7 @@
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6365,7 +6630,7 @@
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6402,7 +6667,7 @@
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6426,8 +6691,8 @@
       <c r="D29" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E29" s="32" t="s">
-        <v>169</v>
+      <c r="E29" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="F29" s="9">
         <f>VLOOKUP(A29,DEPIT!A26:J68,7,0)</f>
@@ -6443,7 +6708,7 @@
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6467,8 +6732,8 @@
       <c r="D30" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>172</v>
+      <c r="E30" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="F30" s="9">
         <f>VLOOKUP(A30,DEPIT!A27:J69,7,0)</f>
@@ -6484,7 +6749,7 @@
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6521,7 +6786,7 @@
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6545,8 +6810,8 @@
       <c r="D32" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="32" t="s">
-        <v>163</v>
+      <c r="E32" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="F32" s="9">
         <f>VLOOKUP(A32,DEPIT!A29:J71,7,0)</f>
@@ -6562,7 +6827,7 @@
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6599,7 +6864,7 @@
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6621,10 +6886,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>176</v>
       </c>
       <c r="F34" s="9">
         <f>VLOOKUP(A34,DEPIT!A31:J73,7,0)</f>
@@ -6640,7 +6905,7 @@
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6662,10 +6927,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>177</v>
       </c>
       <c r="F35" s="9">
         <f>VLOOKUP(A35,DEPIT!A32:J74,7,0)</f>
@@ -6681,7 +6946,7 @@
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-160</v>
+        <v>-166</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6718,7 +6983,7 @@
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6755,7 +7020,7 @@
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6779,8 +7044,8 @@
       <c r="D38" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="32" t="s">
-        <v>177</v>
+      <c r="E38" s="30" t="s">
+        <v>174</v>
       </c>
       <c r="F38" s="9">
         <f>VLOOKUP(A38,DEPIT!A35:J77,7,0)</f>
@@ -6796,7 +7061,7 @@
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6820,8 +7085,8 @@
       <c r="D39" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="32" t="s">
-        <v>170</v>
+      <c r="E39" s="30" t="s">
+        <v>167</v>
       </c>
       <c r="F39" s="9">
         <f>VLOOKUP(A39,DEPIT!A36:J78,7,0)</f>
@@ -6837,7 +7102,7 @@
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6874,7 +7139,7 @@
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6911,7 +7176,7 @@
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6935,8 +7200,8 @@
       <c r="D42" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E42" s="32" t="s">
-        <v>171</v>
+      <c r="E42" s="30" t="s">
+        <v>168</v>
       </c>
       <c r="F42" s="9">
         <f>VLOOKUP(A42,DEPIT!A39:J81,7,0)</f>
@@ -6952,7 +7217,7 @@
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6976,8 +7241,8 @@
       <c r="D43" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E43" s="32" t="s">
-        <v>168</v>
+      <c r="E43" s="30" t="s">
+        <v>165</v>
       </c>
       <c r="F43" s="9">
         <f>VLOOKUP(A43,DEPIT!A40:J82,7,0)</f>
@@ -6993,7 +7258,7 @@
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-125</v>
+        <v>-131</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7030,7 +7295,7 @@
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7067,7 +7332,7 @@
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7104,7 +7369,7 @@
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7128,8 +7393,8 @@
       <c r="D47" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E47" s="32" t="s">
-        <v>169</v>
+      <c r="E47" s="30" t="s">
+        <v>166</v>
       </c>
       <c r="F47" s="9">
         <f>VLOOKUP(A47,DEPIT!A44:J86,7,0)</f>
@@ -7145,7 +7410,7 @@
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44290</v>
+        <v>-44296</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7157,10 +7422,10 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="37"/>
+      <c r="B50" s="35"/>
     </row>
     <row r="51" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
@@ -7196,84 +7461,84 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I5:I47">
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="13" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="24" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="21" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="20" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="15" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="14" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H47">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="1901">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="1901">
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7349,22 +7614,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
@@ -8231,42 +8496,45 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A2:G1048559"/>
+  <dimension ref="A2:G1048569"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="11.5546875" style="7"/>
+    <col min="2" max="2" width="28.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="7"/>
+    <col min="5" max="5" width="35.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11.5546875" style="7"/>
     <col min="10" max="10" width="26.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
@@ -8279,17 +8547,17 @@
         <v>148</v>
       </c>
       <c r="D5" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="30">
+      <c r="A6" s="39">
         <v>6002</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -8301,7 +8569,7 @@
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="30">
+      <c r="A7" s="39">
         <v>6002</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -8310,38 +8578,39 @@
       <c r="C7" s="9">
         <v>45005</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>160</v>
+      <c r="D7" s="31" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="30">
+      <c r="A8" s="39">
+        <v>6002</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="39">
+        <v>6002</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="39">
         <v>6003</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="9">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="30">
-        <v>6003</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="9">
-        <v>45012</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="30">
-        <v>6004</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>150</v>
@@ -8349,51 +8618,50 @@
       <c r="C10" s="9">
         <v>45000</v>
       </c>
-      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="30">
-        <v>6004</v>
+      <c r="A11" s="39">
+        <v>6003</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C11" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>160</v>
+        <v>45012</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="30">
-        <v>6005</v>
+      <c r="A12" s="39">
+        <v>6003</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="C12" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D12" s="8"/>
+        <v>45014</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="30">
-        <v>6005</v>
+      <c r="A13" s="39">
+        <v>6003</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C13" s="9">
-        <v>45005</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>160</v>
+        <v>45026</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="30">
-        <v>6009</v>
+      <c r="A14" s="39">
+        <v>6004</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>150</v>
@@ -8404,185 +8672,201 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="30">
-        <v>6009</v>
+      <c r="A15" s="39">
+        <v>6004</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C15" s="9">
-        <v>45005</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>160</v>
+        <v>45001</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="30">
-        <v>6011</v>
+      <c r="A16" s="39">
+        <v>6004</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="C16" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="30">
-        <v>6011</v>
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="39">
+        <v>6004</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="C17" s="9">
-        <v>45005</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="31">
-        <v>6012</v>
+        <v>45026</v>
+      </c>
+      <c r="D17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="39">
+        <v>6005</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C18" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="30">
-        <v>6013</v>
+        <v>45000</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" s="39">
+        <v>6005</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="9">
+        <v>45005</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" s="39">
+        <v>6005</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="39">
+        <v>6005</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" s="39">
+        <v>6009</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C22" s="9">
         <v>45000</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="31">
-        <v>6014</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C20" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="31">
-        <v>6015</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C21" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="31">
-        <v>6015</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="39">
+        <v>6009</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C22" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="31">
-        <v>6017</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="C23" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="31">
-        <v>6018</v>
+        <v>45005</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="39">
+        <v>6009</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="C24" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="31">
-        <v>6020</v>
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="39">
+        <v>6009</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="C25" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="31">
-        <v>6024</v>
+        <v>45026</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="39">
+        <v>6011</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C26" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="31">
-        <v>6026</v>
+        <v>45000</v>
+      </c>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="39">
+        <v>6011</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C27" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="31">
-        <v>6027</v>
+        <v>45005</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="39">
+        <v>6011</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="C28" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="31">
-        <v>6028</v>
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="39">
+        <v>6011</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="C29" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="31">
-        <v>6029</v>
+        <v>45026</v>
+      </c>
+      <c r="D29" s="31"/>
+      <c r="E29" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="39">
+        <v>6012</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>150</v>
@@ -8591,9 +8875,9 @@
         <v>45001</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="30">
-        <v>6031</v>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" s="39">
+        <v>6013</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>150</v>
@@ -8603,23 +8887,20 @@
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="30">
-        <v>6031</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" s="39">
+        <v>6014</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C32" s="9">
-        <v>45013</v>
-      </c>
-      <c r="D32" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="31">
-        <v>6032</v>
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33" s="39">
+        <v>6015</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>150</v>
@@ -8627,57 +8908,62 @@
       <c r="C33" s="9">
         <v>45001</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" s="31">
-        <v>6033</v>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" s="39">
+        <v>6015</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C34" s="9">
         <v>45001</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" s="31">
-        <v>6034</v>
+      <c r="D34" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35" s="39">
+        <v>6015</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" s="39">
+        <v>6015</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="39">
+        <v>6017</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C37" s="9">
         <v>45001</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="31">
-        <v>6035</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" s="31">
-        <v>6035</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="9">
-        <v>45013</v>
-      </c>
-      <c r="D37" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" s="31">
-        <v>6036</v>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" s="39">
+        <v>6018</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>150</v>
@@ -8685,11 +8971,10 @@
       <c r="C38" s="9">
         <v>45001</v>
       </c>
-      <c r="D38" s="33"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" s="31">
-        <v>6037</v>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39" s="39">
+        <v>6020</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>150</v>
@@ -8697,11 +8982,10 @@
       <c r="C39" s="9">
         <v>45001</v>
       </c>
-      <c r="D39" s="33"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" s="31">
-        <v>6038</v>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" s="39">
+        <v>6024</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>150</v>
@@ -8709,37 +8993,32 @@
       <c r="C40" s="9">
         <v>45001</v>
       </c>
-      <c r="D40" s="33"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" s="30">
-        <v>6039</v>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" s="39">
+        <v>6026</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C41" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D41" s="33"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="30">
-        <v>6039</v>
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" s="39">
+        <v>6027</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C42" s="9">
-        <v>45020</v>
-      </c>
-      <c r="D42" s="33" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" s="31">
-        <v>6040</v>
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="39">
+        <v>6028</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>150</v>
@@ -8747,11 +9026,10 @@
       <c r="C43" s="9">
         <v>45001</v>
       </c>
-      <c r="D43" s="33"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" s="31">
-        <v>6041</v>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="39">
+        <v>6029</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>150</v>
@@ -8759,113 +9037,365 @@
       <c r="C44" s="9">
         <v>45001</v>
       </c>
-      <c r="D44" s="33"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" s="31">
-        <v>6042</v>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="39">
+        <v>6031</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C45" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="39">
+        <v>6031</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="9">
+        <v>45013</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A47" s="39">
+        <v>6031</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48" s="39">
+        <v>6031</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D48" s="31"/>
+      <c r="E48" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A49" s="39">
+        <v>6032</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="9">
         <v>45001</v>
       </c>
-      <c r="D45" s="33"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" s="31">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A50" s="39">
+        <v>6033</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C50" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51" s="39">
+        <v>6034</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52" s="39">
+        <v>6035</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53" s="39">
+        <v>6035</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="9">
+        <v>45013</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54" s="39">
+        <v>6035</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55" s="39">
+        <v>6035</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D55" s="31"/>
+      <c r="E55" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" s="39">
+        <v>6036</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D56" s="31"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57" s="39">
+        <v>6037</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D57" s="31"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58" s="39">
+        <v>6038</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D58" s="31"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59" s="39">
+        <v>6039</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D59" s="31"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60" s="39">
+        <v>6039</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" s="9">
+        <v>45020</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A61" s="39">
+        <v>6039</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" s="9">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62" s="39">
+        <v>6039</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D62" s="31"/>
+      <c r="E62" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63" s="39">
+        <v>6040</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D63" s="31"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64" s="39">
+        <v>6041</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C64" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D64" s="31"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A65" s="39">
+        <v>6042</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D65" s="31"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A66" s="39">
         <v>6043</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B66" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C66" s="9">
         <v>45001</v>
       </c>
-      <c r="D46" s="33"/>
-    </row>
-    <row r="1048552" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048552" s="7" t="s">
+      <c r="D66" s="31"/>
+    </row>
+    <row r="1048562" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048562" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="1048553" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048553" s="29" t="s">
+    <row r="1048563" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048563" s="29" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="1048554" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048554" s="29" t="s">
+    <row r="1048564" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048564" s="29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="1048555" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048555" s="29" t="s">
+    <row r="1048565" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048565" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="1048566" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048566" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1048567" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048567" s="29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1048568" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048568" s="29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="1048556" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048556" s="29" t="s">
+    <row r="1048569" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048569" s="29" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="1048557" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048557" s="29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="1048558" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048558" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="1048559" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048559" s="29" t="s">
-        <v>156</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F46">
-    <sortCondition ref="A6:A46"/>
-    <sortCondition ref="C6:C46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F66">
+    <sortCondition ref="A6:A66"/>
+    <sortCondition ref="C6:C66"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:A15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="A6:A20">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>6043</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:A42">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="A50:A52">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>6043</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B66">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Rectificada / Aprobada">
+      <formula>NOT(ISERROR(SEARCH("Rectificada / Aprobada",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B46" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
-      <formula1>$A$1048553:$A$1048559</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B66" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+      <formula1>$A$1048563:$A$1048569</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" tooltip="6004" xr:uid="{98815502-696A-4ED7-8F42-1713E48F3EEC}"/>
-    <hyperlink ref="D17" r:id="rId2" tooltip="6011" xr:uid="{24D0A05B-C8EE-4787-96DB-2A89DF2B0D89}"/>
+    <hyperlink ref="D15" r:id="rId1" tooltip="6004" xr:uid="{98815502-696A-4ED7-8F42-1713E48F3EEC}"/>
+    <hyperlink ref="D27" r:id="rId2" tooltip="6011" xr:uid="{24D0A05B-C8EE-4787-96DB-2A89DF2B0D89}"/>
     <hyperlink ref="D7" r:id="rId3" tooltip="6002" xr:uid="{214F1D65-92A0-4C91-848F-31097B9C11FD}"/>
-    <hyperlink ref="D13" r:id="rId4" tooltip="6005" xr:uid="{C3CBAD01-E9C1-49F4-A848-4C351A0AC29A}"/>
-    <hyperlink ref="D15" r:id="rId5" tooltip="6009" xr:uid="{41977E1C-88AC-44D4-B0F8-0341DA06AB2C}"/>
-    <hyperlink ref="D22" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
-    <hyperlink ref="D9" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
-    <hyperlink ref="D32" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
-    <hyperlink ref="D37" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
-    <hyperlink ref="D42" r:id="rId10" tooltip="6039" xr:uid="{5CFF6145-29E8-4D14-91C2-F8073B207DDE}"/>
+    <hyperlink ref="D19" r:id="rId4" tooltip="6005" xr:uid="{C3CBAD01-E9C1-49F4-A848-4C351A0AC29A}"/>
+    <hyperlink ref="D23" r:id="rId5" tooltip="6009" xr:uid="{41977E1C-88AC-44D4-B0F8-0341DA06AB2C}"/>
+    <hyperlink ref="D34" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
+    <hyperlink ref="D11" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
+    <hyperlink ref="D46" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
+    <hyperlink ref="D53" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
+    <hyperlink ref="D60" r:id="rId10" tooltip="6039" xr:uid="{5CFF6145-29E8-4D14-91C2-F8073B207DDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>

</xml_diff>

<commit_message>
uucc - envio 3 y 4
</commit_message>
<xml_diff>
--- a/LGTI/0.programas-follow-up.xlsx
+++ b/LGTI/0.programas-follow-up.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\Storage\Dropbox\Documentos\universidad\01.UNPAZ\3.Coordinacion\follow-up-lgti\LGTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B75A83-E1A8-4783-8200-D60079B19D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B05819-FC88-4348-8A70-45ABAB1E5900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F18B9F4F-2FBE-4E7E-BBB1-C1B35DE33D81}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="187">
   <si>
     <t>Análisis Matemático I</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Aprobado</t>
   </si>
   <si>
-    <t>Rectificado</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -618,10 +615,10 @@
     <t>Envío a Desarrollo curricular</t>
   </si>
   <si>
-    <t>Rectificada / Aprobada</t>
-  </si>
-  <si>
     <t>En Modificación</t>
+  </si>
+  <si>
+    <t>Modificada / Aprobada</t>
   </si>
 </sst>
 </file>
@@ -827,7 +824,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -923,7 +920,6 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma" xfId="5" xr:uid="{05F99610-EFDD-41FA-9067-2D9EACE38C58}"/>
@@ -941,14 +937,14 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{561F4419-9779-48EA-98E4-826F7DD662D5}"/>
     <cellStyle name="Percent" xfId="2" xr:uid="{CDE64AD3-5503-4CAE-82E9-E24CD1038088}"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="66">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1039,392 +1035,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
-          <stop position="0">
-            <color theme="0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FFFF0000"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1786,6 +1396,192 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <gradientFill type="path" left="0.5" right="0.5" top="0.5" bottom="0.5">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FFFF0000"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4563,36 +4359,36 @@
     <dataField name="#" fld="9" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
-    <format dxfId="80">
+    <format dxfId="60">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="58">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="57">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="56">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="55">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
+    <format dxfId="54">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4709,23 +4505,23 @@
     <dataField name="Total" fld="0" subtotal="count" baseField="8" baseItem="0"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="85">
+    <format dxfId="65">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="64">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="63">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="8" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4815,29 +4611,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{42237D6D-EEE7-4148-81E3-C70FF28FBFED}" name="Tabla7" displayName="Tabla7" ref="A4:K47" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{00ECA187-D9F9-43F2-A77F-F17D472E5673}" name="CÓDIGO" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{0A440868-BC77-4736-8CAB-DCD16F20C8D8}" name="ASIGNATURA" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{D0EA3073-308D-427B-9EF0-3103F43898D2}" name="AÑO" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{71D14ECB-B5F5-41B2-BF92-78FE3837C54D}" name="PROFESOR" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{3BB31B93-F128-4629-B837-366E0929F1F5}" name="EMAIL" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{C25B3D63-A25E-4473-8D49-76799699482A}" name="INICIO" dataDxfId="27">
       <calculatedColumnFormula>VLOOKUP(A5,DEPIT!A4:J43,7,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="64">
+    <tableColumn id="7" xr3:uid="{119BADE6-ABFE-4E55-A0EA-BE39BDDD1795}" name="DISPO" dataDxfId="26">
       <calculatedColumnFormula>F5+(365*2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="63">
-      <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
+    <tableColumn id="12" xr3:uid="{F8AA8AD4-B821-4480-B8A8-31374D1594FB}" name="VENCE" dataDxfId="25">
+      <calculatedColumnFormula>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="62">
+    <tableColumn id="8" xr3:uid="{C362CEB5-7C81-4357-92FD-B8025B950AD2}" name="SEM" dataDxfId="24">
       <calculatedColumnFormula>G5 - TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="61">
+    <tableColumn id="9" xr3:uid="{06401851-6A3D-4543-B451-27EB95ACE697}" name="ESTADO" dataDxfId="23">
       <calculatedColumnFormula>IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="60">
+    <tableColumn id="11" xr3:uid="{258D018F-27BF-43B6-A2E0-0E9E2AD36868}" name="FULLNAME" dataDxfId="22">
       <calculatedColumnFormula>CONCATENATE(Tabla7[[#This Row],[CÓDIGO]]," - ",Tabla7[[#This Row],[ASIGNATURA]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4846,23 +4642,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}" name="Tabla5" displayName="Tabla5" ref="A4:J49" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A4:J49" xr:uid="{3FA7CDEF-904A-4F74-9A4B-8D9A490790FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:J49">
     <sortCondition ref="A5:A49"/>
     <sortCondition descending="1" ref="G5:G49"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{06335FCA-BB50-454F-A23C-5AE5882E4F8E}" name="Código" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1359A393-A30A-44CC-BE51-39BDA3E1E424}" name="Fecha Aprobación" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{FDDB6F57-FAC5-455E-80A0-C84B84DD99A0}" name="Acta" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{E194A7E7-A329-4857-92AE-8C95993CDFD8}" name="Expediente" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{535E7F8F-CA96-42E8-9530-3FF8800638B5}" name="Nro. Disposición" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A8D71B2D-3EAC-486E-BD13-8885DD48C0C2}" name="Fecha Disposición" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{941F7103-7C81-4EFB-AB69-49EB0D6A103A}" name="Inicio Vigencia" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{BD12D681-160A-45AB-8474-42963C429AEC}" name="Notas" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{1FEBE093-EB0E-4B23-9E0E-A99F5684FA52}" name="CreateOn" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{B65AF4A0-F4EB-4196-A9A2-938224480E33}" name="Estado" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5191,7 +4987,7 @@
   <sheetData>
     <row r="2" spans="1:12" ht="20.399999999999999" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -5201,7 +4997,7 @@
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
       <c r="J2" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K2" s="32"/>
       <c r="L2" s="13">
@@ -5211,7 +5007,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>55</v>
@@ -5219,7 +5015,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="23">
         <v>1</v>
@@ -5227,7 +5023,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="23">
         <v>1</v>
@@ -5235,7 +5031,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="23">
         <v>1</v>
@@ -5243,7 +5039,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="23">
         <v>1</v>
@@ -5251,7 +5047,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="23">
         <v>1</v>
@@ -5259,7 +5055,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="23">
         <v>1</v>
@@ -5268,18 +5064,18 @@
         <v>58</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="23">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="7">
         <v>23</v>
@@ -5287,13 +5083,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="23">
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="7">
         <v>8</v>
@@ -5301,13 +5097,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="23">
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="7">
         <v>12</v>
@@ -5315,7 +5111,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
@@ -5323,7 +5119,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
@@ -5331,7 +5127,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="23">
         <v>1</v>
@@ -5339,7 +5135,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="23">
         <v>1</v>
@@ -5347,7 +5143,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="23">
         <v>1</v>
@@ -5355,7 +5151,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="23">
         <v>1</v>
@@ -5363,7 +5159,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="23">
         <v>1</v>
@@ -5371,7 +5167,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="23">
         <v>1</v>
@@ -5379,7 +5175,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="23">
         <v>1</v>
@@ -5387,7 +5183,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="23">
         <v>1</v>
@@ -5395,7 +5191,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="23">
         <v>1</v>
@@ -5403,7 +5199,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="23">
         <v>1</v>
@@ -5411,7 +5207,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="23">
         <v>1</v>
@@ -5419,7 +5215,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="23">
         <v>1</v>
@@ -5427,7 +5223,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" s="23">
         <v>1</v>
@@ -5435,7 +5231,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="23">
         <v>1</v>
@@ -5443,7 +5239,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="23">
         <v>1</v>
@@ -5451,7 +5247,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="23">
         <v>1</v>
@@ -5459,7 +5255,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="23">
         <v>1</v>
@@ -5467,7 +5263,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="23">
         <v>1</v>
@@ -5475,7 +5271,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="23">
         <v>1</v>
@@ -5483,7 +5279,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" s="23">
         <v>1</v>
@@ -5491,7 +5287,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="23">
         <v>1</v>
@@ -5499,7 +5295,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="23">
         <v>1</v>
@@ -5507,7 +5303,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" s="23">
         <v>1</v>
@@ -5515,7 +5311,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" s="23">
         <v>1</v>
@@ -5523,7 +5319,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" s="23">
         <v>1</v>
@@ -5531,7 +5327,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" s="23">
         <v>1</v>
@@ -5539,7 +5335,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" s="23">
         <v>1</v>
@@ -5547,7 +5343,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" s="23">
         <v>1</v>
@@ -5555,7 +5351,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="23">
         <v>1</v>
@@ -5563,7 +5359,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" s="23">
         <v>1</v>
@@ -5571,7 +5367,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="23">
         <v>1</v>
@@ -5579,7 +5375,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="23">
         <v>1</v>
@@ -5587,7 +5383,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="22">
         <v>43</v>
@@ -5621,8 +5417,8 @@
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -5643,7 +5439,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -5699,19 +5495,19 @@
         <v>57</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>58</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
@@ -5725,26 +5521,26 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F5" s="9">
         <f>VLOOKUP(A5,DEPIT!A4:J43,7,0)</f>
-        <v>44382</v>
+        <v>44697</v>
       </c>
       <c r="G5" s="26">
         <f>F5+(365*2)</f>
-        <v>45112</v>
+        <v>45427</v>
       </c>
       <c r="H5" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>2 Q-2024</v>
       </c>
       <c r="I5" s="11">
         <f ca="1">G5 - TODAY()</f>
-        <v>86</v>
+        <v>383</v>
       </c>
       <c r="J5" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5766,10 +5562,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" s="9">
         <f>VLOOKUP(A6,DEPIT!A5:J44,7,0)</f>
@@ -5780,12 +5576,12 @@
         <v>44895</v>
       </c>
       <c r="H6" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I6" s="11">
         <f t="shared" ref="I6:I47" ca="1" si="0">G6 - TODAY()</f>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J6" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5807,10 +5603,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" s="9">
         <f>VLOOKUP(A7,DEPIT!A6:J45,7,0)</f>
@@ -5821,12 +5617,12 @@
         <v>44895</v>
       </c>
       <c r="H7" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J7" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5848,10 +5644,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F8" s="9">
         <f>VLOOKUP(A8,DEPIT!A7:J46,7,0)</f>
@@ -5862,12 +5658,12 @@
         <v>730</v>
       </c>
       <c r="H8" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J8" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5889,10 +5685,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F9" s="9">
         <f>VLOOKUP(A9,DEPIT!A8:J47,7,0)</f>
@@ -5903,12 +5699,12 @@
         <v>44895</v>
       </c>
       <c r="H9" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J9" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5930,10 +5726,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F10" s="9">
         <f>VLOOKUP(A10,DEPIT!A8:J49,7,0)</f>
@@ -5944,12 +5740,12 @@
         <v>45242</v>
       </c>
       <c r="H10" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J10" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -5971,10 +5767,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F11" s="9">
         <f>VLOOKUP(A11,DEPIT!A8:J50,7,0)</f>
@@ -5985,12 +5781,12 @@
         <v>45242</v>
       </c>
       <c r="H11" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I11" s="11">
         <f ca="1">G11 - TODAY()</f>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J11" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6012,10 +5808,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F12" s="9">
         <f>VLOOKUP(A12,DEPIT!A9:J51,7,0)</f>
@@ -6026,12 +5822,12 @@
         <v>45242</v>
       </c>
       <c r="H12" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J12" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6053,10 +5849,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F13" s="9">
         <f>VLOOKUP(A13,DEPIT!A10:J52,7,0)</f>
@@ -6067,12 +5863,12 @@
         <v>44895</v>
       </c>
       <c r="H13" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J13" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6094,10 +5890,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F14" s="9">
         <f>VLOOKUP(A14,DEPIT!A11:J53,7,0)</f>
@@ -6108,12 +5904,12 @@
         <v>45242</v>
       </c>
       <c r="H14" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J14" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6135,10 +5931,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F15" s="9">
         <f>VLOOKUP(A15,DEPIT!A12:J54,7,0)</f>
@@ -6149,12 +5945,12 @@
         <v>44895</v>
       </c>
       <c r="H15" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J15" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6186,12 +5982,12 @@
         <v>730</v>
       </c>
       <c r="H16" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J16" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6213,10 +6009,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F17" s="9">
         <f>VLOOKUP(A17,DEPIT!A14:J56,7,0)</f>
@@ -6227,12 +6023,12 @@
         <v>44895</v>
       </c>
       <c r="H17" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J17" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6254,10 +6050,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F18" s="9">
         <f>VLOOKUP(A18,DEPIT!A15:J57,7,0)</f>
@@ -6268,12 +6064,12 @@
         <v>730</v>
       </c>
       <c r="H18" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J18" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6295,10 +6091,10 @@
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="9">
         <f>VLOOKUP(A19,DEPIT!A16:J58,7,0)</f>
@@ -6309,12 +6105,12 @@
         <v>730</v>
       </c>
       <c r="H19" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J19" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6336,10 +6132,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F20" s="9">
         <f>VLOOKUP(A20,DEPIT!A17:J59,7,0)</f>
@@ -6350,12 +6146,12 @@
         <v>45435</v>
       </c>
       <c r="H20" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>1 Q-2024</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>2 Q-2024</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="J20" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6377,10 +6173,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F21" s="9">
         <f>VLOOKUP(A21,DEPIT!A18:J60,7,0)</f>
@@ -6391,12 +6187,12 @@
         <v>730</v>
       </c>
       <c r="H21" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J21" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6418,10 +6214,10 @@
         <v>2</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F22" s="9">
         <f>VLOOKUP(A22,DEPIT!A19:J61,7,0)</f>
@@ -6432,12 +6228,12 @@
         <v>730</v>
       </c>
       <c r="H22" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J22" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6459,10 +6255,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F23" s="9">
         <f>VLOOKUP(A23,DEPIT!A20:J62,7,0)</f>
@@ -6473,12 +6269,12 @@
         <v>45427</v>
       </c>
       <c r="H23" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>1 Q-2024</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>2 Q-2024</v>
       </c>
       <c r="I23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="J23" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6510,12 +6306,12 @@
         <v>730</v>
       </c>
       <c r="H24" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J24" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6547,12 +6343,12 @@
         <v>45242</v>
       </c>
       <c r="H25" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J25" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6574,10 +6370,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F26" s="9">
         <f>VLOOKUP(A26,DEPIT!A23:J65,7,0)</f>
@@ -6588,12 +6384,12 @@
         <v>45242</v>
       </c>
       <c r="H26" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J26" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6625,12 +6421,12 @@
         <v>45112</v>
       </c>
       <c r="H27" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="J27" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6662,12 +6458,12 @@
         <v>730</v>
       </c>
       <c r="H28" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J28" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6689,10 +6485,10 @@
         <v>3</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F29" s="9">
         <f>VLOOKUP(A29,DEPIT!A26:J68,7,0)</f>
@@ -6703,12 +6499,12 @@
         <v>45242</v>
       </c>
       <c r="H29" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J29" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6730,10 +6526,10 @@
         <v>3</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F30" s="9">
         <f>VLOOKUP(A30,DEPIT!A27:J69,7,0)</f>
@@ -6744,12 +6540,12 @@
         <v>730</v>
       </c>
       <c r="H30" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J30" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6781,12 +6577,12 @@
         <v>730</v>
       </c>
       <c r="H31" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J31" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6808,10 +6604,10 @@
         <v>3</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F32" s="9">
         <f>VLOOKUP(A32,DEPIT!A29:J71,7,0)</f>
@@ -6822,12 +6618,12 @@
         <v>730</v>
       </c>
       <c r="H32" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J32" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6859,12 +6655,12 @@
         <v>730</v>
       </c>
       <c r="H33" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J33" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6880,16 +6676,16 @@
         <v>6030</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C34" s="8">
         <v>4</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>175</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>176</v>
       </c>
       <c r="F34" s="9">
         <f>VLOOKUP(A34,DEPIT!A31:J73,7,0)</f>
@@ -6900,12 +6696,12 @@
         <v>45242</v>
       </c>
       <c r="H34" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2023</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2023</v>
       </c>
       <c r="I34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="J34" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6927,10 +6723,10 @@
         <v>4</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F35" s="9">
         <f>VLOOKUP(A35,DEPIT!A32:J74,7,0)</f>
@@ -6941,12 +6737,12 @@
         <v>44860</v>
       </c>
       <c r="H35" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-166</v>
+        <v>-184</v>
       </c>
       <c r="J35" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -6978,12 +6774,12 @@
         <v>730</v>
       </c>
       <c r="H36" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J36" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7015,12 +6811,12 @@
         <v>730</v>
       </c>
       <c r="H37" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J37" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7042,10 +6838,10 @@
         <v>4</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F38" s="9">
         <f>VLOOKUP(A38,DEPIT!A35:J77,7,0)</f>
@@ -7056,12 +6852,12 @@
         <v>730</v>
       </c>
       <c r="H38" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J38" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7083,10 +6879,10 @@
         <v>4</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F39" s="9">
         <f>VLOOKUP(A39,DEPIT!A36:J78,7,0)</f>
@@ -7097,12 +6893,12 @@
         <v>730</v>
       </c>
       <c r="H39" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J39" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7134,12 +6930,12 @@
         <v>730</v>
       </c>
       <c r="H40" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J40" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7171,12 +6967,12 @@
         <v>730</v>
       </c>
       <c r="H41" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J41" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7198,10 +6994,10 @@
         <v>4</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F42" s="9">
         <f>VLOOKUP(A42,DEPIT!A39:J81,7,0)</f>
@@ -7212,12 +7008,12 @@
         <v>730</v>
       </c>
       <c r="H42" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J42" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7239,10 +7035,10 @@
         <v>5</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F43" s="9">
         <f>VLOOKUP(A43,DEPIT!A40:J82,7,0)</f>
@@ -7253,12 +7049,12 @@
         <v>44895</v>
       </c>
       <c r="H43" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-2022</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-2022</v>
       </c>
       <c r="I43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-131</v>
+        <v>-149</v>
       </c>
       <c r="J43" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7290,12 +7086,12 @@
         <v>730</v>
       </c>
       <c r="H44" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J44" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7327,12 +7123,12 @@
         <v>730</v>
       </c>
       <c r="H45" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J45" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7364,12 +7160,12 @@
         <v>730</v>
       </c>
       <c r="H46" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J46" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7391,10 +7187,10 @@
         <v>5</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E47" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F47" s="9">
         <f>VLOOKUP(A47,DEPIT!A44:J86,7,0)</f>
@@ -7405,12 +7201,12 @@
         <v>730</v>
       </c>
       <c r="H47" s="24" t="str">
-        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]]) &gt; 6,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
-        <v>2 Q-1901</v>
+        <f>CONCATENATE( IF(MONTH(Tabla7[[#This Row],[DISPO]])  &lt; 7,"2 Q","1 Q"),"-",YEAR(Tabla7[[#This Row],[DISPO]]))</f>
+        <v>1 Q-1901</v>
       </c>
       <c r="I47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>-44296</v>
+        <v>-44314</v>
       </c>
       <c r="J47" s="8" t="str">
         <f ca="1">IF(Tabla7[[#This Row],[SEM]] &gt; 0,"Vigente",IF(Tabla7[[#This Row],[SEM]] &lt; -30000,"Sin presentar","Vencido"))</f>
@@ -7423,26 +7219,26 @@
     </row>
     <row r="50" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B50" s="35"/>
     </row>
     <row r="51" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="5"/>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="6"/>
       <c r="B52" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4"/>
       <c r="B53" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
@@ -7450,7 +7246,7 @@
         <v>45</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -7461,84 +7257,84 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I5:I47">
-    <cfRule type="cellIs" dxfId="47" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="25" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J47">
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="13" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="42" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="21" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F47">
-    <cfRule type="cellIs" dxfId="41" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="40" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="15" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G47">
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="12" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="10" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="lessThan">
       <formula>43466</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="greaterThan">
       <formula>"&gt;01/01/2020"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Vigente"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"Sin presentar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
       <formula>"Vencido"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H47">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="1901">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="1901">
       <formula>NOT(ISERROR(SEARCH("1901",H5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7594,7 +7390,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -7615,7 +7411,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -7624,7 +7420,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -7651,7 +7447,7 @@
         <v>52</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>53</v>
@@ -7660,7 +7456,7 @@
         <v>60</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
@@ -7677,16 +7473,16 @@
         <v>54</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="10">
         <v>44697</v>
       </c>
       <c r="G5" s="10">
-        <v>44382</v>
+        <v>44697</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -7700,10 +7496,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F6" s="10">
         <v>44382</v>
@@ -7729,7 +7525,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="10">
         <v>44165</v>
@@ -7755,7 +7551,7 @@
         <v>56</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" s="10">
         <v>44165</v>
@@ -7789,7 +7585,7 @@
         <v>56</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" s="10">
         <v>44165</v>
@@ -7815,7 +7611,7 @@
         <v>59</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F11" s="10">
         <v>44512</v>
@@ -7841,7 +7637,7 @@
         <v>59</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" s="10">
         <v>44512</v>
@@ -7867,7 +7663,7 @@
         <v>59</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" s="10">
         <v>44512</v>
@@ -7893,7 +7689,7 @@
         <v>56</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F14" s="10">
         <v>44165</v>
@@ -7919,7 +7715,7 @@
         <v>59</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F15" s="10">
         <v>44512</v>
@@ -7945,7 +7741,7 @@
         <v>56</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="10">
         <v>44165</v>
@@ -7982,7 +7778,7 @@
         <v>56</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F18" s="10">
         <v>44165</v>
@@ -8027,10 +7823,10 @@
         <v>31</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="F21" s="10">
         <v>44705</v>
@@ -8078,7 +7874,7 @@
         <v>54</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" s="10">
         <v>44697</v>
@@ -8115,7 +7911,7 @@
         <v>59</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F26" s="10">
         <v>44512</v>
@@ -8141,7 +7937,7 @@
         <v>59</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F27" s="10">
         <v>44512</v>
@@ -8164,10 +7960,10 @@
         <v>24</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F28" s="10">
         <v>44382</v>
@@ -8204,7 +8000,7 @@
         <v>59</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F30" s="10">
         <v>44512</v>
@@ -8274,7 +8070,7 @@
         <v>59</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F35" s="10">
         <v>44512</v>
@@ -8297,10 +8093,10 @@
         <v>19</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F36" s="10">
         <v>44130</v>
@@ -8403,7 +8199,7 @@
         <v>56</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F44" s="10">
         <v>44165</v>
@@ -8496,10 +8292,10 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A2:G1048569"/>
+  <dimension ref="A2:G1048567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -8516,7 +8312,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -8527,7 +8323,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -8538,30 +8334,30 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>58</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="39">
+      <c r="A6" s="7">
         <v>6002</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="9">
         <v>45000</v>
@@ -8569,151 +8365,146 @@
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A7" s="39">
+      <c r="A7" s="7">
         <v>6002</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="9">
         <v>45005</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="39">
+      <c r="A8" s="7">
         <v>6002</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C8" s="9">
         <v>45014</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9" s="39">
+      <c r="A9" s="7">
         <v>6002</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C9" s="9">
         <v>45026</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="39">
-        <v>6003</v>
+      <c r="A10" s="7">
+        <v>6002</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C10" s="9">
-        <v>45000</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11" s="39">
-        <v>6003</v>
+      <c r="A11" s="7">
+        <v>6002</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C11" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="7">
+        <v>6003</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="7">
+        <v>6003</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="9">
         <v>45012</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="39">
+      <c r="D13" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="7">
         <v>6003</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="7">
+        <v>6003</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C12" s="9">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="39">
+      <c r="C15" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="7">
         <v>6003</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C13" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="39">
+      <c r="B16" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" s="7">
+        <v>6003</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" s="7">
         <v>6004</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A15" s="39">
-        <v>6004</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C15" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="39">
-        <v>6004</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="9">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A17" s="39">
-        <v>6004</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D17" s="31"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A18" s="39">
-        <v>6005</v>
-      </c>
       <c r="B18" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C18" s="9">
         <v>45000</v>
@@ -8721,639 +8512,908 @@
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A19" s="39">
-        <v>6005</v>
+      <c r="A19" s="7">
+        <v>6004</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="9">
-        <v>45005</v>
+        <v>45001</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" s="39">
-        <v>6005</v>
+      <c r="A20" s="7">
+        <v>6004</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C20" s="9">
         <v>45014</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A21" s="39">
-        <v>6005</v>
+      <c r="A21" s="7">
+        <v>6004</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C21" s="9">
         <v>45026</v>
       </c>
       <c r="D21" s="31"/>
-      <c r="E21" s="7" t="s">
-        <v>179</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A22" s="39">
+      <c r="A22" s="7">
+        <v>6004</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="9">
+        <v>45005</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D26" s="31"/>
+      <c r="E26" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" s="7">
+        <v>6005</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" s="7">
         <v>6009</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="9">
+      <c r="B29" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="9">
         <v>45000</v>
       </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" s="39">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" s="7">
         <v>6009</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" s="9">
-        <v>45005</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A24" s="39">
-        <v>6009</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24" s="9">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A25" s="39">
-        <v>6009</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A26" s="39">
-        <v>6011</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C26" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A27" s="39">
-        <v>6011</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="9">
-        <v>45005</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A28" s="39">
-        <v>6011</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C28" s="9">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A29" s="39">
-        <v>6011</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C29" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A30" s="39">
-        <v>6012</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C30" s="9">
-        <v>45001</v>
+        <v>45005</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A31" s="39">
-        <v>6013</v>
+      <c r="A31" s="7">
+        <v>6009</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="C31" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D31" s="8"/>
+        <v>45014</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A32" s="39">
-        <v>6014</v>
+      <c r="A32" s="7">
+        <v>6009</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="C32" s="9">
-        <v>45001</v>
+        <v>45026</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A33" s="39">
-        <v>6015</v>
+      <c r="A33" s="7">
+        <v>6009</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C33" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D33" s="8"/>
+        <v>45030</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" s="39">
-        <v>6015</v>
+      <c r="A34" s="7">
+        <v>6009</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C34" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>157</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A35" s="39">
-        <v>6015</v>
+      <c r="A35" s="7">
+        <v>6011</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" s="7">
+        <v>6011</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="9">
+        <v>45005</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="7">
+        <v>6011</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" s="7">
+        <v>6011</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C35" s="9">
-        <v>45014</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A36" s="39">
-        <v>6015</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="C36" s="9">
+      <c r="C38" s="9">
         <v>45026</v>
       </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A37" s="39">
-        <v>6017</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="9">
-        <v>45001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A38" s="39">
-        <v>6018</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C38" s="9">
-        <v>45001</v>
+      <c r="D38" s="31"/>
+      <c r="E38" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A39" s="39">
-        <v>6020</v>
+      <c r="A39" s="7">
+        <v>6011</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="C39" s="9">
-        <v>45001</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A40" s="39">
-        <v>6024</v>
+      <c r="A40" s="7">
+        <v>6011</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C40" s="9">
-        <v>45001</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A41" s="39">
-        <v>6026</v>
+      <c r="A41" s="7">
+        <v>6012</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C41" s="9">
         <v>45001</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A42" s="39">
-        <v>6027</v>
+      <c r="A42" s="7">
+        <v>6013</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" s="9">
-        <v>45001</v>
-      </c>
+        <v>45000</v>
+      </c>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A43" s="39">
-        <v>6028</v>
+      <c r="A43" s="7">
+        <v>6014</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="9">
         <v>45001</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A44" s="39">
-        <v>6029</v>
+      <c r="A44" s="7">
+        <v>6015</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="9">
         <v>45001</v>
       </c>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A45" s="39">
-        <v>6031</v>
+      <c r="A45" s="7">
+        <v>6015</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C45" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D45" s="8"/>
+        <v>45001</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A46" s="39">
-        <v>6031</v>
+      <c r="A46" s="7">
+        <v>6015</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="C46" s="9">
-        <v>45013</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>157</v>
+        <v>45014</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A47" s="39">
-        <v>6031</v>
+      <c r="A47" s="7">
+        <v>6015</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>185</v>
       </c>
       <c r="C47" s="9">
-        <v>45014</v>
+        <v>45026</v>
+      </c>
+      <c r="D47" s="31"/>
+      <c r="E47" s="7" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A48" s="39">
-        <v>6031</v>
+      <c r="A48" s="7">
+        <v>6015</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C48" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="7" t="s">
-        <v>182</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A49" s="39">
-        <v>6032</v>
+      <c r="A49" s="7">
+        <v>6015</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C49" s="9">
-        <v>45001</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A50" s="39">
-        <v>6033</v>
+      <c r="A50" s="7">
+        <v>6017</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" s="9">
         <v>45001</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A51" s="39">
-        <v>6034</v>
+      <c r="A51" s="7">
+        <v>6018</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C51" s="9">
         <v>45001</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A52" s="39">
-        <v>6035</v>
+      <c r="A52" s="7">
+        <v>6020</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" s="9">
         <v>45001</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A53" s="39">
-        <v>6035</v>
+      <c r="A53" s="7">
+        <v>6024</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C53" s="9">
-        <v>45013</v>
-      </c>
-      <c r="D53" s="31" t="s">
-        <v>157</v>
+        <v>45001</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A54" s="39">
-        <v>6035</v>
+      <c r="A54" s="7">
+        <v>6026</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="C54" s="9">
-        <v>45014</v>
+        <v>45001</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A55" s="39">
-        <v>6035</v>
+      <c r="A55" s="7">
+        <v>6027</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="C55" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="7" t="s">
-        <v>183</v>
+        <v>45001</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A56" s="39">
-        <v>6036</v>
+      <c r="A56" s="7">
+        <v>6028</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C56" s="9">
         <v>45001</v>
       </c>
-      <c r="D56" s="31"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A57" s="39">
-        <v>6037</v>
+      <c r="A57" s="7">
+        <v>6029</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="9">
         <v>45001</v>
       </c>
-      <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A58" s="39">
-        <v>6038</v>
+      <c r="A58" s="7">
+        <v>6031</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D58" s="31"/>
+        <v>45000</v>
+      </c>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A59" s="39">
-        <v>6039</v>
+      <c r="A59" s="7">
+        <v>6031</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>150</v>
       </c>
       <c r="C59" s="9">
-        <v>45000</v>
-      </c>
-      <c r="D59" s="31"/>
+        <v>45013</v>
+      </c>
+      <c r="D59" s="31" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A60" s="39">
-        <v>6039</v>
+      <c r="A60" s="7">
+        <v>6031</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
       <c r="C60" s="9">
-        <v>45020</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>157</v>
+        <v>45014</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A61" s="39">
-        <v>6039</v>
+      <c r="A61" s="7">
+        <v>6031</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>185</v>
       </c>
       <c r="C61" s="9">
-        <v>45020</v>
+        <v>45026</v>
+      </c>
+      <c r="D61" s="31"/>
+      <c r="E61" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A62" s="39">
-        <v>6039</v>
+      <c r="A62" s="7">
+        <v>6031</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C62" s="9">
-        <v>45026</v>
-      </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="7" t="s">
-        <v>184</v>
+        <v>45030</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A63" s="39">
-        <v>6040</v>
+      <c r="A63" s="7">
+        <v>6031</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C63" s="9">
-        <v>45001</v>
-      </c>
-      <c r="D63" s="31"/>
+        <v>45030</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A64" s="39">
-        <v>6041</v>
+      <c r="A64" s="7">
+        <v>6032</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C64" s="9">
         <v>45001</v>
       </c>
-      <c r="D64" s="31"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A65" s="39">
-        <v>6042</v>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A65" s="7">
+        <v>6033</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C65" s="9">
         <v>45001</v>
       </c>
-      <c r="D65" s="31"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A66" s="39">
-        <v>6043</v>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A66" s="7">
+        <v>6034</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C66" s="9">
         <v>45001</v>
       </c>
-      <c r="D66" s="31"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A67" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="9">
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A68" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="9">
+        <v>45013</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A69" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" s="9">
+        <v>45014</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A70" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D70" s="31"/>
+      <c r="E70" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A71" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C71" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A72" s="7">
+        <v>6035</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C72" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A73" s="7">
+        <v>6036</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C73" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D73" s="31"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A74" s="7">
+        <v>6037</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D74" s="31"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A75" s="7">
+        <v>6038</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D75" s="31"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A76" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" s="9">
+        <v>45000</v>
+      </c>
+      <c r="D76" s="31"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A77" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77" s="9">
+        <v>45020</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A78" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" s="9">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A79" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" s="9">
+        <v>45026</v>
+      </c>
+      <c r="D79" s="31"/>
+      <c r="E79" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A80" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C80" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A81" s="7">
+        <v>6039</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C81" s="9">
+        <v>45030</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A82" s="7">
+        <v>6040</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C82" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D82" s="31"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A83" s="7">
+        <v>6041</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C83" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D83" s="31"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A84" s="7">
+        <v>6042</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C84" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D84" s="31"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A85" s="7">
+        <v>6043</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C85" s="9">
+        <v>45001</v>
+      </c>
+      <c r="D85" s="31"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A86" s="7">
+        <v>6043</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" s="9">
+        <v>45027</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A87" s="7">
+        <v>6026</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C87" s="9">
+        <v>45041</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A88" s="7">
+        <v>6027</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="9">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A89" s="7">
+        <v>6033</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C89" s="9">
+        <v>45043</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A90" s="7">
+        <v>6014</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90" s="9">
+        <v>45044</v>
+      </c>
+    </row>
+    <row r="1048560" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048560" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="1048561" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1048561" s="29" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="1048562" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048562" s="7" t="s">
-        <v>149</v>
+      <c r="A1048562" s="29" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="1048563" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048563" s="29" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
     </row>
     <row r="1048564" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048564" s="29" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
     </row>
     <row r="1048565" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048565" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="1048566" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048566" s="29" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
     </row>
     <row r="1048567" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1048567" s="29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="1048568" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048568" s="29" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="1048569" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A1048569" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F66">
-    <sortCondition ref="A6:A66"/>
-    <sortCondition ref="C6:C66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:F85">
+    <sortCondition ref="A6:A85"/>
+    <sortCondition ref="C6:C85"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
@@ -9367,7 +9427,7 @@
       <formula>6043</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:A52">
+  <conditionalFormatting sqref="A49:A51">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>6001</formula>
     </cfRule>
@@ -9375,29 +9435,47 @@
       <formula>6043</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B66">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Rectificada / Aprobada">
-      <formula>NOT(ISERROR(SEARCH("Rectificada / Aprobada",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B66" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
-      <formula1>$A$1048563:$A$1048569</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B90" xr:uid="{BCD53E5E-82D4-4741-8401-3537DA9A8231}">
+      <formula1>$A$1048561:$A$1048567</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" tooltip="6004" xr:uid="{98815502-696A-4ED7-8F42-1713E48F3EEC}"/>
-    <hyperlink ref="D27" r:id="rId2" tooltip="6011" xr:uid="{24D0A05B-C8EE-4787-96DB-2A89DF2B0D89}"/>
+    <hyperlink ref="D19" r:id="rId1" tooltip="6004" xr:uid="{98815502-696A-4ED7-8F42-1713E48F3EEC}"/>
+    <hyperlink ref="D36" r:id="rId2" tooltip="6011" xr:uid="{24D0A05B-C8EE-4787-96DB-2A89DF2B0D89}"/>
     <hyperlink ref="D7" r:id="rId3" tooltip="6002" xr:uid="{214F1D65-92A0-4C91-848F-31097B9C11FD}"/>
-    <hyperlink ref="D19" r:id="rId4" tooltip="6005" xr:uid="{C3CBAD01-E9C1-49F4-A848-4C351A0AC29A}"/>
-    <hyperlink ref="D23" r:id="rId5" tooltip="6009" xr:uid="{41977E1C-88AC-44D4-B0F8-0341DA06AB2C}"/>
-    <hyperlink ref="D34" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
-    <hyperlink ref="D11" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
-    <hyperlink ref="D46" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
-    <hyperlink ref="D53" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
-    <hyperlink ref="D60" r:id="rId10" tooltip="6039" xr:uid="{5CFF6145-29E8-4D14-91C2-F8073B207DDE}"/>
+    <hyperlink ref="D24" r:id="rId4" tooltip="6005" xr:uid="{C3CBAD01-E9C1-49F4-A848-4C351A0AC29A}"/>
+    <hyperlink ref="D30" r:id="rId5" tooltip="6009" xr:uid="{41977E1C-88AC-44D4-B0F8-0341DA06AB2C}"/>
+    <hyperlink ref="D45" r:id="rId6" tooltip="6015" xr:uid="{75F51838-4752-4571-BFA9-D830EE100EB6}"/>
+    <hyperlink ref="D13" r:id="rId7" tooltip="6003" xr:uid="{B59295BE-7431-4B0B-A29E-F10C045106BA}"/>
+    <hyperlink ref="D59" r:id="rId8" tooltip="6031" xr:uid="{A92D7A6D-8709-4F87-A778-68C9EB0CAAE7}"/>
+    <hyperlink ref="D68" r:id="rId9" tooltip="6035" xr:uid="{36531DB0-50C0-4DA6-9ED7-89AE1C2F3F66}"/>
+    <hyperlink ref="D77" r:id="rId10" tooltip="6039" xr:uid="{5CFF6145-29E8-4D14-91C2-F8073B207DDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{6CC1EC41-DEC5-496E-B047-E9631C889C3F}">
+            <xm:f>NOT(ISERROR(SEARCH($A$1048565,B6)))</xm:f>
+            <xm:f>$A$1048565</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0" tint="-0.14996795556505021"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B6:B90</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>